<commit_message>
Adicionando estrategias para reduzir resistencias dos membros do projeto.
</commit_message>
<xml_diff>
--- a/docs/Documentos/Registro_das_partes_interessadas.xlsx
+++ b/docs/Documentos/Registro_das_partes_interessadas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\talit\OneDrive\Documentos\GitHub\if-map\docs\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manri\OneDrive\Documentos\Github\if-map\docs\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE176ED7-6A1B-4902-A5CC-14FD46C2545F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F157C615-BEC1-4409-A15F-8B209D2182D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="81">
   <si>
     <t>Registro das partes interessadas</t>
   </si>
@@ -192,9 +192,6 @@
   </si>
   <si>
     <t>1-Muito baixo</t>
-  </si>
-  <si>
-    <t>Delegar ou fazer</t>
   </si>
   <si>
     <t>Matriz de Poder x Interesse</t>
@@ -288,7 +285,176 @@
     <t xml:space="preserve">A conclusão com exito maximo </t>
   </si>
   <si>
-    <t>Auxiliar e concluir as tarefas do semestre</t>
+    <r>
+      <t xml:space="preserve">Auxiliar e concluir as tarefas do semestre / </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">reuniões para introduzi-lo ao projeto </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">/ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ser acessível</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ouvir ideias e sujestões </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">/ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">receber feedback positivo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">/ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">deixar claro das espectativias sobre ele </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">/ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>incentiva-lo a tomar decisões importantes do projeto.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Com o time trabalhando em grupo me sinto mais motivado em continuar no projeto. / </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ser acessível.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Delegar ou fazer / </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ser acessível </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>receber feedback positivo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>deixar claro das espectativias sobre ele.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -298,7 +464,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mmm/yyyy"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -457,11 +623,15 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="23">
@@ -782,7 +952,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="35" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="35" applyFont="1"/>
@@ -886,9 +1056,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -919,22 +1086,33 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="35" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" xfId="35" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="38" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="35" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="38" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="38" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="35" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -942,27 +1120,11 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="35" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="35" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="38" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="38" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" xfId="35" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="38" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="35" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="38" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -978,7 +1140,18 @@
     <xf numFmtId="0" fontId="2" fillId="20" borderId="2" xfId="38" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="39">
     <cellStyle name="Accent1 - 20%" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -1590,13 +1763,13 @@
         <v>4</v>
       </c>
       <c r="E5" s="18"/>
-      <c r="F5" s="74" t="s">
+      <c r="F5" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
     </row>
     <row r="6" spans="1:10" s="14" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="15"/>
@@ -1636,90 +1809,90 @@
       <c r="B10" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
     </row>
     <row r="11" spans="1:10" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="76" t="s">
+      <c r="C11" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76" t="s">
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="76"/>
-      <c r="I11" s="77" t="s">
+      <c r="H11" s="65"/>
+      <c r="I11" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="77"/>
+      <c r="J11" s="66"/>
     </row>
     <row r="12" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="27">
         <v>1</v>
       </c>
-      <c r="C12" s="71" t="s">
+      <c r="C12" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="72" t="s">
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="72"/>
-      <c r="I12" s="73"/>
-      <c r="J12" s="73"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="69"/>
     </row>
     <row r="13" spans="1:10" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="27">
         <f>B12+1</f>
         <v>2</v>
       </c>
-      <c r="C13" s="71" t="s">
+      <c r="C13" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="72" t="s">
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="72"/>
-      <c r="I13" s="73"/>
-      <c r="J13" s="73"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="69"/>
     </row>
     <row r="14" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="69"/>
-      <c r="I14" s="70"/>
-      <c r="J14" s="70"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="71"/>
+      <c r="H14" s="71"/>
+      <c r="I14" s="72"/>
+      <c r="J14" s="72"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:10" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="66"/>
-      <c r="I16" s="66"/>
-      <c r="J16" s="66"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="73"/>
+      <c r="I16" s="73"/>
+      <c r="J16" s="73"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="28" t="s">
@@ -1731,50 +1904,50 @@
       <c r="D17" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="67" t="s">
+      <c r="E17" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="74"/>
+      <c r="J17" s="74"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="65"/>
-      <c r="J18" s="65"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="75"/>
+      <c r="I18" s="75"/>
+      <c r="J18" s="75"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="65"/>
-      <c r="I19" s="65"/>
-      <c r="J19" s="65"/>
+      <c r="E19" s="75"/>
+      <c r="F19" s="75"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="75"/>
+      <c r="I19" s="75"/>
+      <c r="J19" s="75"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25"/>
     <row r="21" spans="2:10" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B21" s="66" t="s">
+      <c r="B21" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="66"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="66"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="66"/>
-      <c r="I21" s="66"/>
-      <c r="J21" s="66"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="73"/>
+      <c r="H21" s="73"/>
+      <c r="I21" s="73"/>
+      <c r="J21" s="73"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="28" t="s">
@@ -1786,14 +1959,14 @@
       <c r="D22" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="67" t="s">
+      <c r="E22" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="67"/>
-      <c r="G22" s="67"/>
-      <c r="H22" s="67"/>
-      <c r="I22" s="67"/>
-      <c r="J22" s="67"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="74"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="74"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="29">
@@ -1801,12 +1974,12 @@
       </c>
       <c r="C23" s="29"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="65"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="65"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75"/>
+      <c r="I23" s="75"/>
+      <c r="J23" s="75"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="29">
@@ -1814,12 +1987,12 @@
       </c>
       <c r="C24" s="29"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="65"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="75"/>
+      <c r="J24" s="75"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25"/>
@@ -1847,28 +2020,28 @@
     <row r="48" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="B21:J21"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="B16:J16"/>
+    <mergeCell ref="E17:J17"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="I13:J13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="B16:J16"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E18:J18"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="B21:J21"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" location="Capa!A1" display="Capa" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -1894,10 +2067,10 @@
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="M4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M6" sqref="M6"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1937,20 +2110,20 @@
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="32"/>
-      <c r="D2" s="78" t="s">
+      <c r="D2" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="79" t="s">
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
       <c r="N2" s="36"/>
       <c r="P2" s="33"/>
     </row>
@@ -2006,38 +2179,40 @@
         <f t="shared" ref="C4:C29" si="0">IF(ISTEXT(L4),LEFT(L4,1),L4)*IF(ISTEXT(M4),LEFT(M4,1),M4)</f>
         <v>5</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="41">
+      <c r="F4" s="60">
         <v>84992296101</v>
       </c>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41" t="s">
+      <c r="G4" s="60" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="41" t="s">
+      <c r="I4" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="41" t="s">
+      <c r="J4" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="41" t="s">
+      <c r="K4" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="L4" s="44" t="s">
+      <c r="L4" s="81" t="s">
         <v>46</v>
       </c>
-      <c r="M4" s="44" t="s">
+      <c r="M4" s="81" t="s">
         <v>47</v>
       </c>
       <c r="N4" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="O4" s="45"/>
+        <v>80</v>
+      </c>
+      <c r="O4" s="44"/>
     </row>
     <row r="5" spans="2:16" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="41">
@@ -2048,82 +2223,86 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="D5" s="62" t="s">
+      <c r="D5" s="60" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="63" t="s">
+      <c r="F5" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="F5" s="61" t="s">
+      <c r="G5" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="62" t="s">
+      <c r="H5" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="H5" s="62" t="s">
+      <c r="I5" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="60" t="s">
         <v>71</v>
       </c>
-      <c r="I5" s="62" t="s">
+      <c r="K5" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="L5" s="81" t="s">
+        <v>46</v>
+      </c>
+      <c r="M5" s="81" t="s">
+        <v>64</v>
+      </c>
+      <c r="N5" s="82" t="s">
+        <v>79</v>
+      </c>
+      <c r="O5" s="44"/>
+    </row>
+    <row r="6" spans="2:16" s="45" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B6" s="41">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="C6" s="42">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="60" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="62" t="s">
-        <v>72</v>
-      </c>
-      <c r="K5" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="L5" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="M5" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="N5" s="64"/>
-      <c r="O5" s="45"/>
-    </row>
-    <row r="6" spans="2:16" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="41">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="C6" s="42">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="D6" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="83" t="s">
-        <v>75</v>
-      </c>
-      <c r="F6" s="41" t="s">
+      <c r="J6" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" s="41" t="s">
+      <c r="K6" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="K6" s="41" t="s">
+      <c r="L6" s="81" t="s">
+        <v>64</v>
+      </c>
+      <c r="M6" s="81" t="s">
+        <v>64</v>
+      </c>
+      <c r="N6" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="L6" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="M6" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="N6" s="41" t="s">
-        <v>79</v>
-      </c>
       <c r="O6" s="41"/>
     </row>
-    <row r="7" spans="2:16" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="41">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -2140,12 +2319,12 @@
       <c r="I7" s="41"/>
       <c r="J7" s="41"/>
       <c r="K7" s="41"/>
-      <c r="L7" s="44"/>
-      <c r="M7" s="44"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
       <c r="N7" s="41"/>
       <c r="O7" s="41"/>
     </row>
-    <row r="8" spans="2:16" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="41">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -2162,12 +2341,12 @@
       <c r="I8" s="41"/>
       <c r="J8" s="41"/>
       <c r="K8" s="41"/>
-      <c r="L8" s="44"/>
-      <c r="M8" s="44"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
       <c r="N8" s="41"/>
       <c r="O8" s="41"/>
     </row>
-    <row r="9" spans="2:16" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="41">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -2184,12 +2363,12 @@
       <c r="I9" s="41"/>
       <c r="J9" s="41"/>
       <c r="K9" s="41"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="44"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
       <c r="N9" s="41"/>
       <c r="O9" s="41"/>
     </row>
-    <row r="10" spans="2:16" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="41">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -2206,12 +2385,12 @@
       <c r="I10" s="41"/>
       <c r="J10" s="41"/>
       <c r="K10" s="41"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
       <c r="N10" s="41"/>
       <c r="O10" s="41"/>
     </row>
-    <row r="11" spans="2:16" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="41">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -2228,12 +2407,12 @@
       <c r="I11" s="41"/>
       <c r="J11" s="41"/>
       <c r="K11" s="41"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="44"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
       <c r="N11" s="41"/>
       <c r="O11" s="41"/>
     </row>
-    <row r="12" spans="2:16" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="41">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -2250,12 +2429,12 @@
       <c r="I12" s="41"/>
       <c r="J12" s="41"/>
       <c r="K12" s="41"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="44"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
       <c r="N12" s="41"/>
       <c r="O12" s="41"/>
     </row>
-    <row r="13" spans="2:16" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="41">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -2272,12 +2451,12 @@
       <c r="I13" s="41"/>
       <c r="J13" s="41"/>
       <c r="K13" s="41"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="44"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
       <c r="N13" s="41"/>
       <c r="O13" s="41"/>
     </row>
-    <row r="14" spans="2:16" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="41">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -2294,12 +2473,12 @@
       <c r="I14" s="41"/>
       <c r="J14" s="41"/>
       <c r="K14" s="41"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="44"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
       <c r="N14" s="41"/>
       <c r="O14" s="41"/>
     </row>
-    <row r="15" spans="2:16" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="41">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -2316,12 +2495,12 @@
       <c r="I15" s="41"/>
       <c r="J15" s="41"/>
       <c r="K15" s="41"/>
-      <c r="L15" s="44"/>
-      <c r="M15" s="44"/>
-      <c r="N15" s="45"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="44"/>
       <c r="O15" s="41"/>
     </row>
-    <row r="16" spans="2:16" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="41">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -2338,12 +2517,12 @@
       <c r="I16" s="41"/>
       <c r="J16" s="41"/>
       <c r="K16" s="41"/>
-      <c r="L16" s="44"/>
-      <c r="M16" s="44"/>
-      <c r="N16" s="45"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="43"/>
+      <c r="N16" s="44"/>
       <c r="O16" s="41"/>
     </row>
-    <row r="17" spans="2:15" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="41">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -2360,12 +2539,12 @@
       <c r="I17" s="41"/>
       <c r="J17" s="41"/>
       <c r="K17" s="41"/>
-      <c r="L17" s="44"/>
-      <c r="M17" s="44"/>
-      <c r="N17" s="45"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="44"/>
       <c r="O17" s="41"/>
     </row>
-    <row r="18" spans="2:15" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="41">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -2382,12 +2561,12 @@
       <c r="I18" s="41"/>
       <c r="J18" s="41"/>
       <c r="K18" s="41"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="44"/>
-      <c r="N18" s="45"/>
+      <c r="L18" s="43"/>
+      <c r="M18" s="43"/>
+      <c r="N18" s="44"/>
       <c r="O18" s="41"/>
     </row>
-    <row r="19" spans="2:15" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="41">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -2404,12 +2583,12 @@
       <c r="I19" s="41"/>
       <c r="J19" s="41"/>
       <c r="K19" s="41"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="44"/>
-      <c r="N19" s="45"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="44"/>
       <c r="O19" s="41"/>
     </row>
-    <row r="20" spans="2:15" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="41">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -2426,12 +2605,12 @@
       <c r="I20" s="41"/>
       <c r="J20" s="41"/>
       <c r="K20" s="41"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="44"/>
-      <c r="N20" s="45"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="44"/>
       <c r="O20" s="41"/>
     </row>
-    <row r="21" spans="2:15" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="41">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -2448,12 +2627,12 @@
       <c r="I21" s="41"/>
       <c r="J21" s="41"/>
       <c r="K21" s="41"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="44"/>
-      <c r="N21" s="45"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="44"/>
       <c r="O21" s="41"/>
     </row>
-    <row r="22" spans="2:15" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="41">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -2470,12 +2649,12 @@
       <c r="I22" s="41"/>
       <c r="J22" s="41"/>
       <c r="K22" s="41"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="45"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="44"/>
       <c r="O22" s="41"/>
     </row>
-    <row r="23" spans="2:15" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="41">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -2492,12 +2671,12 @@
       <c r="I23" s="41"/>
       <c r="J23" s="41"/>
       <c r="K23" s="41"/>
-      <c r="L23" s="44"/>
-      <c r="M23" s="44"/>
-      <c r="N23" s="45"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="44"/>
       <c r="O23" s="41"/>
     </row>
-    <row r="24" spans="2:15" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="41">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -2514,12 +2693,12 @@
       <c r="I24" s="41"/>
       <c r="J24" s="41"/>
       <c r="K24" s="41"/>
-      <c r="L24" s="44"/>
-      <c r="M24" s="44"/>
-      <c r="N24" s="45"/>
+      <c r="L24" s="43"/>
+      <c r="M24" s="43"/>
+      <c r="N24" s="44"/>
       <c r="O24" s="41"/>
     </row>
-    <row r="25" spans="2:15" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="41">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -2536,12 +2715,12 @@
       <c r="I25" s="41"/>
       <c r="J25" s="41"/>
       <c r="K25" s="41"/>
-      <c r="L25" s="44"/>
-      <c r="M25" s="44"/>
-      <c r="N25" s="45"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="44"/>
       <c r="O25" s="41"/>
     </row>
-    <row r="26" spans="2:15" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:15" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="41">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -2558,12 +2737,12 @@
       <c r="I26" s="41"/>
       <c r="J26" s="41"/>
       <c r="K26" s="41"/>
-      <c r="L26" s="44"/>
-      <c r="M26" s="44"/>
-      <c r="N26" s="45"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="44"/>
       <c r="O26" s="41"/>
     </row>
-    <row r="27" spans="2:15" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:15" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="41">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -2580,12 +2759,12 @@
       <c r="I27" s="41"/>
       <c r="J27" s="41"/>
       <c r="K27" s="41"/>
-      <c r="L27" s="44"/>
-      <c r="M27" s="44"/>
-      <c r="N27" s="45"/>
+      <c r="L27" s="43"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="44"/>
       <c r="O27" s="41"/>
     </row>
-    <row r="28" spans="2:15" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:15" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="41">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -2602,12 +2781,12 @@
       <c r="I28" s="41"/>
       <c r="J28" s="41"/>
       <c r="K28" s="41"/>
-      <c r="L28" s="44"/>
-      <c r="M28" s="44"/>
-      <c r="N28" s="45"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="43"/>
+      <c r="N28" s="44"/>
       <c r="O28" s="41"/>
     </row>
-    <row r="29" spans="2:15" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:15" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="41">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -2624,9 +2803,9 @@
       <c r="I29" s="41"/>
       <c r="J29" s="41"/>
       <c r="K29" s="41"/>
-      <c r="L29" s="44"/>
-      <c r="M29" s="44"/>
-      <c r="N29" s="45"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="43"/>
+      <c r="N29" s="44"/>
       <c r="O29" s="41"/>
     </row>
     <row r="30" spans="2:15" s="30" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2691,68 +2870,68 @@
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D2" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="30" t="s">
         <v>49</v>
-      </c>
-      <c r="L2" s="30" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J3" s="30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="K4" s="79" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="K4" s="81" t="s">
+      <c r="L4" s="79"/>
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="79"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="J5" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="L4" s="81"/>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="J5" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="K5" s="45">
+      <c r="K5" s="44">
         <v>1</v>
       </c>
-      <c r="L5" s="45">
+      <c r="L5" s="44">
         <f>K5+1</f>
         <v>2</v>
       </c>
-      <c r="M5" s="45">
+      <c r="M5" s="44">
         <f>L5+1</f>
         <v>3</v>
       </c>
-      <c r="N5" s="45">
+      <c r="N5" s="44">
         <f>M5+1</f>
         <v>4</v>
       </c>
-      <c r="O5" s="45">
+      <c r="O5" s="44">
         <f>N5+1</f>
         <v>5</v>
       </c>
-      <c r="P5" s="49" t="s">
-        <v>54</v>
+      <c r="P5" s="48" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="45">
+      <c r="B6" s="44">
         <f>B7+1</f>
         <v>5</v>
       </c>
@@ -2776,8 +2955,8 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="H6" s="50"/>
-      <c r="J6" s="45">
+      <c r="H6" s="49"/>
+      <c r="J6" s="44">
         <f>J7+1</f>
         <v>5</v>
       </c>
@@ -2801,13 +2980,13 @@
         <f t="shared" si="1"/>
         <v>625</v>
       </c>
-      <c r="P6" s="45">
+      <c r="P6" s="44">
         <f>P7+1</f>
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="45">
+      <c r="B7" s="44">
         <f>B8+1</f>
         <v>4</v>
       </c>
@@ -2831,8 +3010,8 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="H7" s="50"/>
-      <c r="J7" s="45">
+      <c r="H7" s="49"/>
+      <c r="J7" s="44">
         <f>J8+1</f>
         <v>4</v>
       </c>
@@ -2856,13 +3035,13 @@
         <f t="shared" si="1"/>
         <v>400</v>
       </c>
-      <c r="P7" s="45">
+      <c r="P7" s="44">
         <f>P8+1</f>
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="45">
+      <c r="B8" s="44">
         <f>B9+1</f>
         <v>3</v>
       </c>
@@ -2886,8 +3065,8 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H8" s="50"/>
-      <c r="J8" s="45">
+      <c r="H8" s="49"/>
+      <c r="J8" s="44">
         <f>J9+1</f>
         <v>3</v>
       </c>
@@ -2911,13 +3090,13 @@
         <f t="shared" si="1"/>
         <v>225</v>
       </c>
-      <c r="P8" s="45">
+      <c r="P8" s="44">
         <f>P9+1</f>
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="45">
+      <c r="B9" s="44">
         <f>B10+1</f>
         <v>2</v>
       </c>
@@ -2941,8 +3120,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="H9" s="50"/>
-      <c r="J9" s="45">
+      <c r="H9" s="49"/>
+      <c r="J9" s="44">
         <f>J10+1</f>
         <v>2</v>
       </c>
@@ -2966,13 +3145,13 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="P9" s="45">
+      <c r="P9" s="44">
         <f>P10+1</f>
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="45">
+      <c r="B10" s="44">
         <v>1</v>
       </c>
       <c r="C10" s="30">
@@ -2995,8 +3174,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H10" s="50"/>
-      <c r="J10" s="45">
+      <c r="H10" s="49"/>
+      <c r="J10" s="44">
         <v>1</v>
       </c>
       <c r="K10" s="30">
@@ -3019,65 +3198,65 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="P10" s="45">
+      <c r="P10" s="44">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C11" s="45">
+      <c r="C11" s="44">
         <v>1</v>
       </c>
-      <c r="D11" s="45">
+      <c r="D11" s="44">
         <f>C11+1</f>
         <v>2</v>
       </c>
-      <c r="E11" s="45">
+      <c r="E11" s="44">
         <f>D11+1</f>
         <v>3</v>
       </c>
-      <c r="F11" s="45">
+      <c r="F11" s="44">
         <f>E11+1</f>
         <v>4</v>
       </c>
-      <c r="G11" s="45">
+      <c r="G11" s="44">
         <f>F11+1</f>
         <v>5</v>
       </c>
-      <c r="K11" s="45">
+      <c r="K11" s="44">
         <v>1</v>
       </c>
-      <c r="L11" s="45">
+      <c r="L11" s="44">
         <f>K11+1</f>
         <v>2</v>
       </c>
-      <c r="M11" s="45">
+      <c r="M11" s="44">
         <f>L11+1</f>
         <v>3</v>
       </c>
-      <c r="N11" s="45">
+      <c r="N11" s="44">
         <f>M11+1</f>
         <v>4</v>
       </c>
-      <c r="O11" s="45">
+      <c r="O11" s="44">
         <f>N11+1</f>
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C12" s="81" t="s">
+      <c r="C12" s="79" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="79"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="79"/>
+      <c r="K12" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="81"/>
-      <c r="E12" s="81"/>
-      <c r="F12" s="81"/>
-      <c r="G12" s="81"/>
-      <c r="K12" s="81" t="s">
-        <v>55</v>
-      </c>
-      <c r="L12" s="81"/>
-      <c r="M12" s="81"/>
-      <c r="N12" s="81"/>
-      <c r="O12" s="81"/>
+      <c r="L12" s="79"/>
+      <c r="M12" s="79"/>
+      <c r="N12" s="79"/>
+      <c r="O12" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3139,99 +3318,99 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="80" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+    </row>
+    <row r="3" spans="2:6" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-    </row>
-    <row r="3" spans="2:6" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="51" t="s">
+      <c r="C3" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="51" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="B4" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="52" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="52" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="52" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="52" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="B4" s="53" t="s">
+      <c r="C4" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="D4" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="55" t="s">
+      <c r="E4" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="F4" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="54" t="s">
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="55" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="56" t="s">
+      <c r="C5" s="52"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="52" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="49"/>
+      <c r="C6" s="57"/>
+      <c r="E6" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="53" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="53" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="50"/>
-      <c r="C6" s="58"/>
-      <c r="E6" s="58" t="s">
+      <c r="F6" s="57" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="49"/>
+      <c r="C7" s="57"/>
+      <c r="E7" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="58" t="s">
+      <c r="F7" s="57" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="50"/>
-      <c r="C7" s="58"/>
-      <c r="E7" s="58" t="s">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="49"/>
+      <c r="C8" s="57"/>
+      <c r="E8" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="58" t="s">
+      <c r="F8" s="57" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="50"/>
-      <c r="C8" s="58"/>
-      <c r="E8" s="58" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="58" t="s">
-        <v>66</v>
-      </c>
-    </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="59"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="60" t="s">
+      <c r="B9" s="58"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="60" t="s">
+      <c r="F9" s="59" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionando parte interessada coordenador
</commit_message>
<xml_diff>
--- a/docs/Documentos/Registro_das_partes_interessadas.xlsx
+++ b/docs/Documentos/Registro_das_partes_interessadas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manri\OneDrive\Documentos\Github\if-map\docs\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F157C615-BEC1-4409-A15F-8B209D2182D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF878911-07E5-4FCD-919C-FF634D1DBBBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="87">
   <si>
     <t>Registro das partes interessadas</t>
   </si>
@@ -455,6 +455,24 @@
       </rPr>
       <t>deixar claro das espectativias sobre ele.</t>
     </r>
+  </si>
+  <si>
+    <t>Francisco sales filho</t>
+  </si>
+  <si>
+    <t>salesfilho@gmail.com</t>
+  </si>
+  <si>
+    <t>IFRN</t>
+  </si>
+  <si>
+    <t>Coordenador</t>
+  </si>
+  <si>
+    <t>Orientar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cosiguir atingir os objetivos do projeto. </t>
   </si>
 </sst>
 </file>
@@ -1092,27 +1110,23 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="35" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="38" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="38" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="35" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" xfId="35" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="38" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="35" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1120,11 +1134,27 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="35" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" xfId="35" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="38" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="35" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="35" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="38" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="38" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="38" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1139,18 +1169,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="2" xfId="38" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="39">
@@ -1763,13 +1781,13 @@
         <v>4</v>
       </c>
       <c r="E5" s="18"/>
-      <c r="F5" s="63" t="s">
+      <c r="F5" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
     </row>
     <row r="6" spans="1:10" s="14" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="15"/>
@@ -1809,66 +1827,66 @@
       <c r="B10" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="64" t="s">
+      <c r="C10" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="77"/>
     </row>
     <row r="11" spans="1:10" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="65" t="s">
+      <c r="C11" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="65" t="s">
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="65"/>
-      <c r="I11" s="66" t="s">
+      <c r="H11" s="78"/>
+      <c r="I11" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="66"/>
+      <c r="J11" s="79"/>
     </row>
     <row r="12" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="27">
         <v>1</v>
       </c>
-      <c r="C12" s="67" t="s">
+      <c r="C12" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="67"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="68" t="s">
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="68"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="69"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="75"/>
+      <c r="J12" s="75"/>
     </row>
     <row r="13" spans="1:10" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="27">
         <f>B12+1</f>
         <v>2</v>
       </c>
-      <c r="C13" s="67" t="s">
+      <c r="C13" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="68" t="s">
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="68"/>
-      <c r="I13" s="69"/>
-      <c r="J13" s="69"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75"/>
     </row>
     <row r="14" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C14" s="70"/>
@@ -1882,17 +1900,17 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:10" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B16" s="73" t="s">
+      <c r="B16" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="73"/>
-      <c r="I16" s="73"/>
-      <c r="J16" s="73"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="68"/>
+      <c r="J16" s="68"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="28" t="s">
@@ -1904,50 +1922,50 @@
       <c r="D17" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="74" t="s">
+      <c r="E17" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="74"/>
-      <c r="J17" s="74"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="69"/>
+      <c r="H17" s="69"/>
+      <c r="I17" s="69"/>
+      <c r="J17" s="69"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="75"/>
-      <c r="I18" s="75"/>
-      <c r="J18" s="75"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="75"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25"/>
     <row r="21" spans="2:10" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B21" s="73" t="s">
+      <c r="B21" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="73"/>
-      <c r="D21" s="73"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="73"/>
-      <c r="G21" s="73"/>
-      <c r="H21" s="73"/>
-      <c r="I21" s="73"/>
-      <c r="J21" s="73"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="68"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="68"/>
+      <c r="J21" s="68"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="28" t="s">
@@ -1959,14 +1977,14 @@
       <c r="D22" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="74" t="s">
+      <c r="E22" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="74"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="69"/>
+      <c r="I22" s="69"/>
+      <c r="J22" s="69"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="29">
@@ -1974,12 +1992,12 @@
       </c>
       <c r="C23" s="29"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="75"/>
-      <c r="F23" s="75"/>
-      <c r="G23" s="75"/>
-      <c r="H23" s="75"/>
-      <c r="I23" s="75"/>
-      <c r="J23" s="75"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="67"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="29">
@@ -1987,12 +2005,12 @@
       </c>
       <c r="C24" s="29"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="75"/>
-      <c r="H24" s="75"/>
-      <c r="I24" s="75"/>
-      <c r="J24" s="75"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="67"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25"/>
@@ -2020,28 +2038,28 @@
     <row r="48" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="B16:J16"/>
+    <mergeCell ref="E17:J17"/>
     <mergeCell ref="E24:J24"/>
     <mergeCell ref="E18:J18"/>
     <mergeCell ref="E19:J19"/>
     <mergeCell ref="B21:J21"/>
     <mergeCell ref="E22:J22"/>
     <mergeCell ref="E23:J23"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="B16:J16"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" location="Capa!A1" display="Capa" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2070,7 +2088,7 @@
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2110,20 +2128,20 @@
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="32"/>
-      <c r="D2" s="76" t="s">
+      <c r="D2" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="77" t="s">
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
       <c r="N2" s="36"/>
       <c r="P2" s="33"/>
     </row>
@@ -2182,7 +2200,7 @@
       <c r="D4" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="83" t="s">
+      <c r="E4" s="65" t="s">
         <v>41</v>
       </c>
       <c r="F4" s="60">
@@ -2200,13 +2218,13 @@
       <c r="J4" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="84" t="s">
+      <c r="K4" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="L4" s="81" t="s">
+      <c r="L4" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="M4" s="81" t="s">
+      <c r="M4" s="63" t="s">
         <v>47</v>
       </c>
       <c r="N4" s="41" t="s">
@@ -2247,13 +2265,13 @@
       <c r="K5" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="L5" s="81" t="s">
+      <c r="L5" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="81" t="s">
+      <c r="M5" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="N5" s="82" t="s">
+      <c r="N5" s="64" t="s">
         <v>79</v>
       </c>
       <c r="O5" s="44"/>
@@ -2288,13 +2306,13 @@
       <c r="J6" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="K6" s="82" t="s">
+      <c r="K6" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="L6" s="81" t="s">
+      <c r="L6" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="M6" s="81" t="s">
+      <c r="M6" s="63" t="s">
         <v>64</v>
       </c>
       <c r="N6" s="41" t="s">
@@ -2302,25 +2320,45 @@
       </c>
       <c r="O6" s="41"/>
     </row>
-    <row r="7" spans="2:16" s="45" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="41">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C7" s="42">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="43"/>
+        <v>20</v>
+      </c>
+      <c r="D7" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="60" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" s="60" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="I7" s="60" t="s">
+        <v>84</v>
+      </c>
+      <c r="J7" s="60" t="s">
+        <v>85</v>
+      </c>
+      <c r="K7" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="L7" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="M7" s="43" t="s">
+        <v>46</v>
+      </c>
       <c r="N7" s="41"/>
       <c r="O7" s="41"/>
     </row>
@@ -2840,9 +2878,10 @@
     <hyperlink ref="E4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="E5" r:id="rId2" xr:uid="{BF5D3AA4-1238-4650-B399-B401726FC921}"/>
     <hyperlink ref="E6" r:id="rId3" display="marc.viniciusg@gmail.com" xr:uid="{261D932B-B1FC-4991-BBB6-34EE5E869A15}"/>
+    <hyperlink ref="E7" r:id="rId4" xr:uid="{C148EFD2-4CA2-4FB8-9046-F7A57C3A92C6}"/>
   </hyperlinks>
   <pageMargins left="0.23611111111111099" right="0.31527777777777799" top="0.59027777777777801" bottom="0.78749999999999998" header="0.118055555555556" footer="0.31527777777777799"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Calibri,Regular"&amp;11Registro e plano de gerenciamento das partes interessadas&amp;R&amp;"Calibri,Regular"&amp;11&amp;A</oddHeader>
     <oddFooter>&amp;L&amp;"Calibri,Regular"&amp;11&amp;F
@@ -2882,18 +2921,18 @@
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="K4" s="79" t="s">
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="K4" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="L4" s="79"/>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="79"/>
+      <c r="L4" s="83"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="83"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="46" t="s">
@@ -3243,20 +3282,20 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C12" s="79" t="s">
+      <c r="C12" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="79"/>
-      <c r="E12" s="79"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="79"/>
-      <c r="K12" s="79" t="s">
+      <c r="D12" s="83"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="83"/>
+      <c r="G12" s="83"/>
+      <c r="K12" s="83" t="s">
         <v>54</v>
       </c>
-      <c r="L12" s="79"/>
-      <c r="M12" s="79"/>
-      <c r="N12" s="79"/>
-      <c r="O12" s="79"/>
+      <c r="L12" s="83"/>
+      <c r="M12" s="83"/>
+      <c r="N12" s="83"/>
+      <c r="O12" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3318,13 +3357,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
     </row>
     <row r="3" spans="2:6" s="37" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="50" t="s">

</xml_diff>

<commit_message>
doc: adicionada parte interessada de Mozart
</commit_message>
<xml_diff>
--- a/docs/Documentos/Registro_das_partes_interessadas.xlsx
+++ b/docs/Documentos/Registro_das_partes_interessadas.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manri\OneDrive\Documentos\Github\if-map\docs\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\dev\pds\if-map\docs\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF878911-07E5-4FCD-919C-FF634D1DBBBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
     <definedName name="Poder">Param!$E$5:$E$9</definedName>
     <definedName name="t">{"'TG'!$A$1:$L$37"}</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -48,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="93">
   <si>
     <t>Registro das partes interessadas</t>
   </si>
@@ -474,11 +473,29 @@
   <si>
     <t xml:space="preserve">Cosiguir atingir os objetivos do projeto. </t>
   </si>
+  <si>
+    <t>Mozart Orleans Domingos R. Maia</t>
+  </si>
+  <si>
+    <t>mozartmaia89@gmail.com</t>
+  </si>
+  <si>
+    <t>84 996659132</t>
+  </si>
+  <si>
+    <t>Dev. Frontend</t>
+  </si>
+  <si>
+    <t>Auxiliar nas tarefas e entregar qualidade ao projeto.</t>
+  </si>
+  <si>
+    <t>Fazer as tarefas do projeto. Estar disponível para reuniões e feedback quando necessário. Se comunicar com o time.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mmm/yyyy"/>
   </numFmts>
@@ -1122,11 +1139,27 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="35" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" xfId="35" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="38" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="35" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="38" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="38" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="35" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1134,27 +1167,11 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="35" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="35" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="35" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="38" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="38" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" xfId="35" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="38" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="35" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="38" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1172,45 +1189,45 @@
     </xf>
   </cellXfs>
   <cellStyles count="39">
-    <cellStyle name="Accent1 - 20%" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Accent1 - 20% 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Accent1 - 40%" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Accent1 - 40% 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Accent1 - 60%" xfId="6" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Accent2 - 20%" xfId="7" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Accent2 - 20% 2" xfId="8" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Accent2 - 40%" xfId="9" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="Accent2 - 40% 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="Accent2 - 60%" xfId="11" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="Accent3 - 20%" xfId="12" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="Accent3 - 20% 2" xfId="13" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Accent3 - 40%" xfId="14" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Accent3 - 40% 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Accent3 - 60%" xfId="16" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="Accent4 - 20%" xfId="17" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Accent4 - 20% 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Accent4 - 40%" xfId="19" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="Accent4 - 40% 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="Accent4 - 60%" xfId="21" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Accent5 - 20%" xfId="22" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Accent5 - 20% 2" xfId="23" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="Accent5 - 40%" xfId="24" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Accent5 - 40% 2" xfId="25" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="Accent5 - 60%" xfId="26" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="Accent6 - 20%" xfId="27" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="Accent6 - 20% 2" xfId="28" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="Accent6 - 40%" xfId="29" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Accent6 - 40% 2" xfId="30" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="Accent6 - 60%" xfId="31" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Emphasis 1" xfId="32" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Emphasis 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Emphasis 3" xfId="34" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="Excel Built-in Accent1" xfId="38" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Accent1 - 20%" xfId="2"/>
+    <cellStyle name="Accent1 - 20% 2" xfId="3"/>
+    <cellStyle name="Accent1 - 40%" xfId="4"/>
+    <cellStyle name="Accent1 - 40% 2" xfId="5"/>
+    <cellStyle name="Accent1 - 60%" xfId="6"/>
+    <cellStyle name="Accent2 - 20%" xfId="7"/>
+    <cellStyle name="Accent2 - 20% 2" xfId="8"/>
+    <cellStyle name="Accent2 - 40%" xfId="9"/>
+    <cellStyle name="Accent2 - 40% 2" xfId="10"/>
+    <cellStyle name="Accent2 - 60%" xfId="11"/>
+    <cellStyle name="Accent3 - 20%" xfId="12"/>
+    <cellStyle name="Accent3 - 20% 2" xfId="13"/>
+    <cellStyle name="Accent3 - 40%" xfId="14"/>
+    <cellStyle name="Accent3 - 40% 2" xfId="15"/>
+    <cellStyle name="Accent3 - 60%" xfId="16"/>
+    <cellStyle name="Accent4 - 20%" xfId="17"/>
+    <cellStyle name="Accent4 - 20% 2" xfId="18"/>
+    <cellStyle name="Accent4 - 40%" xfId="19"/>
+    <cellStyle name="Accent4 - 40% 2" xfId="20"/>
+    <cellStyle name="Accent4 - 60%" xfId="21"/>
+    <cellStyle name="Accent5 - 20%" xfId="22"/>
+    <cellStyle name="Accent5 - 20% 2" xfId="23"/>
+    <cellStyle name="Accent5 - 40%" xfId="24"/>
+    <cellStyle name="Accent5 - 40% 2" xfId="25"/>
+    <cellStyle name="Accent5 - 60%" xfId="26"/>
+    <cellStyle name="Accent6 - 20%" xfId="27"/>
+    <cellStyle name="Accent6 - 20% 2" xfId="28"/>
+    <cellStyle name="Accent6 - 40%" xfId="29"/>
+    <cellStyle name="Accent6 - 40% 2" xfId="30"/>
+    <cellStyle name="Accent6 - 60%" xfId="31"/>
+    <cellStyle name="Emphasis 1" xfId="32"/>
+    <cellStyle name="Emphasis 2" xfId="33"/>
+    <cellStyle name="Emphasis 3" xfId="34"/>
+    <cellStyle name="Excel Built-in Accent1" xfId="38"/>
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Percent 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="Sheet Title" xfId="37" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Normal 2" xfId="35"/>
+    <cellStyle name="Percent 2" xfId="36"/>
+    <cellStyle name="Sheet Title" xfId="37"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -1702,7 +1719,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ48"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -1781,13 +1798,13 @@
         <v>4</v>
       </c>
       <c r="E5" s="18"/>
-      <c r="F5" s="76" t="s">
+      <c r="F5" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="76"/>
-      <c r="H5" s="76"/>
-      <c r="I5" s="76"/>
-      <c r="J5" s="76"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
     </row>
     <row r="6" spans="1:10" s="14" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="15"/>
@@ -1827,90 +1844,90 @@
       <c r="B10" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="77" t="s">
+      <c r="C10" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="77"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="77"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
     </row>
     <row r="11" spans="1:10" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="78" t="s">
+      <c r="C11" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="78"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="78" t="s">
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="78"/>
-      <c r="I11" s="79" t="s">
+      <c r="H11" s="69"/>
+      <c r="I11" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="79"/>
+      <c r="J11" s="70"/>
     </row>
     <row r="12" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="27">
         <v>1</v>
       </c>
-      <c r="C12" s="73" t="s">
+      <c r="C12" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="74" t="s">
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="74"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="75"/>
+      <c r="H12" s="72"/>
+      <c r="I12" s="73"/>
+      <c r="J12" s="73"/>
     </row>
     <row r="13" spans="1:10" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="27">
         <f>B12+1</f>
         <v>2</v>
       </c>
-      <c r="C13" s="73" t="s">
+      <c r="C13" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="74" t="s">
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="74"/>
-      <c r="I13" s="75"/>
-      <c r="J13" s="75"/>
+      <c r="H13" s="72"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
     </row>
     <row r="14" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="C14" s="70"/>
-      <c r="D14" s="70"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="71"/>
-      <c r="H14" s="71"/>
-      <c r="I14" s="72"/>
-      <c r="J14" s="72"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="75"/>
+      <c r="H14" s="75"/>
+      <c r="I14" s="76"/>
+      <c r="J14" s="76"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:10" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B16" s="68" t="s">
+      <c r="B16" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="68"/>
-      <c r="H16" s="68"/>
-      <c r="I16" s="68"/>
-      <c r="J16" s="68"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="77"/>
+      <c r="H16" s="77"/>
+      <c r="I16" s="77"/>
+      <c r="J16" s="77"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="28" t="s">
@@ -1922,50 +1939,50 @@
       <c r="D17" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="69" t="s">
+      <c r="E17" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="69"/>
-      <c r="G17" s="69"/>
-      <c r="H17" s="69"/>
-      <c r="I17" s="69"/>
-      <c r="J17" s="69"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="78"/>
+      <c r="I17" s="78"/>
+      <c r="J17" s="78"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="67"/>
-      <c r="G18" s="67"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="67"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="79"/>
+      <c r="J18" s="79"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="67"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="67"/>
-      <c r="H19" s="67"/>
-      <c r="I19" s="67"/>
-      <c r="J19" s="67"/>
+      <c r="E19" s="79"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="79"/>
+      <c r="I19" s="79"/>
+      <c r="J19" s="79"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25"/>
     <row r="21" spans="2:10" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B21" s="68" t="s">
+      <c r="B21" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="68"/>
-      <c r="D21" s="68"/>
-      <c r="E21" s="68"/>
-      <c r="F21" s="68"/>
-      <c r="G21" s="68"/>
-      <c r="H21" s="68"/>
-      <c r="I21" s="68"/>
-      <c r="J21" s="68"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="77"/>
+      <c r="H21" s="77"/>
+      <c r="I21" s="77"/>
+      <c r="J21" s="77"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="28" t="s">
@@ -1977,14 +1994,14 @@
       <c r="D22" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="69" t="s">
+      <c r="E22" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="69"/>
-      <c r="G22" s="69"/>
-      <c r="H22" s="69"/>
-      <c r="I22" s="69"/>
-      <c r="J22" s="69"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="78"/>
+      <c r="I22" s="78"/>
+      <c r="J22" s="78"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="29">
@@ -1992,12 +2009,12 @@
       </c>
       <c r="C23" s="29"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="67"/>
-      <c r="H23" s="67"/>
-      <c r="I23" s="67"/>
-      <c r="J23" s="67"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="79"/>
+      <c r="J23" s="79"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="29">
@@ -2005,12 +2022,12 @@
       </c>
       <c r="C24" s="29"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="67"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="67"/>
-      <c r="J24" s="67"/>
+      <c r="E24" s="79"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="79"/>
+      <c r="J24" s="79"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25"/>
@@ -2038,35 +2055,35 @@
     <row r="48" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="E24:J24"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="B21:J21"/>
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="B16:J16"/>
+    <mergeCell ref="E17:J17"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="I13:J13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="B16:J16"/>
-    <mergeCell ref="E17:J17"/>
-    <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E18:J18"/>
-    <mergeCell ref="E19:J19"/>
-    <mergeCell ref="B21:J21"/>
-    <mergeCell ref="E22:J22"/>
-    <mergeCell ref="E23:J23"/>
+    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D4" location="Capa!A1" display="Capa" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D5" location="PartesInteressadas!A1" display="Partes interessadas" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D6" location="Param!A1" display="Parâmetros" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="G12" location="PartesInteressadas!A1" display="Partes Interessadas" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G13" location="PartesInteressadas!A1" display="Partes Interessadas" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D4" location="Capa!A1" display="Capa"/>
+    <hyperlink ref="D5" location="PartesInteressadas!A1" display="Partes interessadas"/>
+    <hyperlink ref="D6" location="Param!A1" display="Parâmetros"/>
+    <hyperlink ref="G12" location="PartesInteressadas!A1" display="Partes Interessadas"/>
+    <hyperlink ref="G13" location="PartesInteressadas!A1" display="Partes Interessadas"/>
   </hyperlinks>
   <pageMargins left="0.23611111111111099" right="0.31527777777777799" top="0.59027777777777801" bottom="0.78749999999999998" header="0.118055555555556" footer="0.31527777777777799"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -2081,14 +2098,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2362,26 +2379,46 @@
       <c r="N7" s="41"/>
       <c r="O7" s="41"/>
     </row>
-    <row r="8" spans="2:16" s="45" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" s="45" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="41">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C8" s="42">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
+        <v>9</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="62" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" s="41" t="s">
+        <v>89</v>
+      </c>
       <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="43"/>
-      <c r="N8" s="41"/>
+      <c r="H8" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="K8" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="L8" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="M8" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="N8" s="41" t="s">
+        <v>92</v>
+      </c>
       <c r="O8" s="41"/>
     </row>
     <row r="9" spans="2:16" s="45" customFormat="1" x14ac:dyDescent="0.25">
@@ -2865,23 +2902,24 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L4:L29" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L4:L29">
       <formula1>Poder</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="M4:M29" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="M4:M29">
       <formula1>Interesse</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="E5" r:id="rId2" xr:uid="{BF5D3AA4-1238-4650-B399-B401726FC921}"/>
-    <hyperlink ref="E6" r:id="rId3" display="marc.viniciusg@gmail.com" xr:uid="{261D932B-B1FC-4991-BBB6-34EE5E869A15}"/>
-    <hyperlink ref="E7" r:id="rId4" xr:uid="{C148EFD2-4CA2-4FB8-9046-F7A57C3A92C6}"/>
+    <hyperlink ref="E4" r:id="rId1"/>
+    <hyperlink ref="E5" r:id="rId2"/>
+    <hyperlink ref="E6" r:id="rId3" display="marc.viniciusg@gmail.com"/>
+    <hyperlink ref="E7" r:id="rId4"/>
+    <hyperlink ref="E8" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.23611111111111099" right="0.31527777777777799" top="0.59027777777777801" bottom="0.78749999999999998" header="0.118055555555556" footer="0.31527777777777799"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Calibri,Regular"&amp;11Registro e plano de gerenciamento das partes interessadas&amp;R&amp;"Calibri,Regular"&amp;11&amp;A</oddHeader>
     <oddFooter>&amp;L&amp;"Calibri,Regular"&amp;11&amp;F
@@ -2892,7 +2930,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AMJ12"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -3338,7 +3376,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AMJ9"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">

</xml_diff>